<commit_message>
12 May 2020 World Report, Russia, India, USA, Bangladesh
World Covid Status Report 12 May 2020, United States Status, Internet Foundation
https://youtu.be/Qb7e5luytEc
</commit_message>
<xml_diff>
--- a/Analyses/Bangladesh 10 May 2020 Cases Deaths and Constant Battle Scenario.xlsx
+++ b/Analyses/Bangladesh 10 May 2020 Cases Deaths and Constant Battle Scenario.xlsx
@@ -12,10 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11232"/>
   </bookViews>
   <sheets>
-    <sheet name="ECDC Case Death Sheet for Curve" sheetId="1" r:id="rId1"/>
+    <sheet name="Bangladesh" sheetId="1" r:id="rId1"/>
+    <sheet name="Population by Age and Sex" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'ECDC Case Death Sheet for Curve'!$P$1:$P$3</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Bangladesh!$P$1:$P$3</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -29,7 +30,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'ECDC Case Death Sheet for Curve'!$P$4</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Bangladesh!$P$4</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
@@ -43,12 +44,12 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t>Bangladesh</t>
   </si>
@@ -79,17 +80,174 @@
   <si>
     <t>Est Cumul Deaths</t>
   </si>
+  <si>
+    <t>2010 - 2011</t>
+  </si>
+  <si>
+    <t>&lt; 5</t>
+  </si>
+  <si>
+    <t>&gt;60</t>
+  </si>
+  <si>
+    <t>2011 - 2012</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5818342/</t>
+  </si>
+  <si>
+    <t>influenza-associated mortality in Bangladesh</t>
+  </si>
+  <si>
+    <t>Age Group</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>0-4</t>
+  </si>
+  <si>
+    <t>15-19</t>
+  </si>
+  <si>
+    <t>20-24</t>
+  </si>
+  <si>
+    <t>25-29</t>
+  </si>
+  <si>
+    <t>30-34</t>
+  </si>
+  <si>
+    <t>35-39</t>
+  </si>
+  <si>
+    <t>40-44</t>
+  </si>
+  <si>
+    <t>45-49</t>
+  </si>
+  <si>
+    <t>50-54</t>
+  </si>
+  <si>
+    <t>55-59</t>
+  </si>
+  <si>
+    <t>60-64</t>
+  </si>
+  <si>
+    <t>65-69</t>
+  </si>
+  <si>
+    <t>70-74</t>
+  </si>
+  <si>
+    <t>75-79</t>
+  </si>
+  <si>
+    <t>80-84</t>
+  </si>
+  <si>
+    <t>85-89</t>
+  </si>
+  <si>
+    <t>90-94</t>
+  </si>
+  <si>
+    <t>95+</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Demographics_of_Bangladesh</t>
+  </si>
+  <si>
+    <t>60+</t>
+  </si>
+  <si>
+    <t>Per 1 000 000</t>
+  </si>
+  <si>
+    <t>Persons</t>
+  </si>
+  <si>
+    <t>Est Persons</t>
+  </si>
+  <si>
+    <t>million</t>
+  </si>
+  <si>
+    <t>&lt;5</t>
+  </si>
+  <si>
+    <t>per month</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/22511823/</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/22271960/</t>
+  </si>
+  <si>
+    <t>Season in months</t>
+  </si>
+  <si>
+    <t>5 - 59</t>
+  </si>
+  <si>
+    <t>2009 - 2010</t>
+  </si>
+  <si>
+    <t>per year</t>
+  </si>
+  <si>
+    <t>5 - 9</t>
+  </si>
+  <si>
+    <t>10-14</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>% Total</t>
+  </si>
+  <si>
+    <t>Pop 2017</t>
+  </si>
+  <si>
+    <t>Per Million</t>
+  </si>
+  <si>
+    <t>https://www.worldlifeexpectancy.com/bangladesh-influenza-pneumonia</t>
+  </si>
+  <si>
+    <t>Tot Deaths</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,8 +382,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -423,6 +589,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -555,7 +733,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -599,14 +777,59 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="35" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="36" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="16" fillId="37" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="33" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="37" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
@@ -641,6 +864,7 @@
     <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
     <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
@@ -745,7 +969,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$B$6</c:f>
+              <c:f>Bangladesh!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -768,7 +992,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$A$7:$A$62</c:f>
+              <c:f>Bangladesh!$A$7:$A$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -945,7 +1169,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$B$7:$B$62</c:f>
+              <c:f>Bangladesh!$B$7:$B$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -1127,7 +1351,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$C$6</c:f>
+              <c:f>Bangladesh!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1150,7 +1374,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$A$7:$A$62</c:f>
+              <c:f>Bangladesh!$A$7:$A$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -1327,7 +1551,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$C$7:$C$62</c:f>
+              <c:f>Bangladesh!$C$7:$C$62</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="56"/>
@@ -1512,11 +1736,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="419598024"/>
-        <c:axId val="419596456"/>
+        <c:axId val="347363584"/>
+        <c:axId val="347367112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="419598024"/>
+        <c:axId val="347363584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40"/>
@@ -1574,12 +1798,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="419596456"/>
+        <c:crossAx val="347367112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="419596456"/>
+        <c:axId val="347367112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,7 +1860,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="419598024"/>
+        <c:crossAx val="347363584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1798,7 +2022,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$D$6</c:f>
+              <c:f>Bangladesh!$D$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1821,7 +2045,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$A$7:$A$62</c:f>
+              <c:f>Bangladesh!$A$7:$A$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -1998,7 +2222,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$D$7:$D$62</c:f>
+              <c:f>Bangladesh!$D$7:$D$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -2180,7 +2404,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$E$6</c:f>
+              <c:f>Bangladesh!$E$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2203,7 +2427,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$A$7:$A$62</c:f>
+              <c:f>Bangladesh!$A$7:$A$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -2380,7 +2604,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$E$7:$E$62</c:f>
+              <c:f>Bangladesh!$E$7:$E$62</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="56"/>
@@ -2565,11 +2789,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="419603120"/>
-        <c:axId val="352222384"/>
+        <c:axId val="347361624"/>
+        <c:axId val="347364760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="419603120"/>
+        <c:axId val="347361624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40"/>
@@ -2627,12 +2851,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="352222384"/>
+        <c:crossAx val="347364760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="352222384"/>
+        <c:axId val="347364760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2689,7 +2913,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="419603120"/>
+        <c:crossAx val="347361624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2856,7 +3080,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$G$6</c:f>
+              <c:f>Bangladesh!$G$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2879,7 +3103,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$F$7:$F$62</c:f>
+              <c:f>Bangladesh!$F$7:$F$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -3056,7 +3280,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$G$7:$G$62</c:f>
+              <c:f>Bangladesh!$G$7:$G$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -3238,7 +3462,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$H$6</c:f>
+              <c:f>Bangladesh!$H$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3261,7 +3485,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$F$7:$F$62</c:f>
+              <c:f>Bangladesh!$F$7:$F$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -3438,7 +3662,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$H$7:$H$62</c:f>
+              <c:f>Bangladesh!$H$7:$H$62</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="56"/>
@@ -3623,11 +3847,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="419602728"/>
-        <c:axId val="419601552"/>
+        <c:axId val="347362408"/>
+        <c:axId val="347365936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="419602728"/>
+        <c:axId val="347362408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40"/>
@@ -3685,12 +3909,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="419601552"/>
+        <c:crossAx val="347365936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="419601552"/>
+        <c:axId val="347365936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3747,7 +3971,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="419602728"/>
+        <c:crossAx val="347362408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3914,7 +4138,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$I$6</c:f>
+              <c:f>Bangladesh!$I$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3937,7 +4161,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$F$7:$F$62</c:f>
+              <c:f>Bangladesh!$F$7:$F$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -4114,7 +4338,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$I$7:$I$62</c:f>
+              <c:f>Bangladesh!$I$7:$I$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -4296,7 +4520,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$J$6</c:f>
+              <c:f>Bangladesh!$J$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4319,7 +4543,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$F$7:$F$62</c:f>
+              <c:f>Bangladesh!$F$7:$F$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -4496,7 +4720,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$J$7:$J$62</c:f>
+              <c:f>Bangladesh!$J$7:$J$62</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="56"/>
@@ -4681,11 +4905,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="352221992"/>
-        <c:axId val="427371696"/>
+        <c:axId val="347368288"/>
+        <c:axId val="347368680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="352221992"/>
+        <c:axId val="347368288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40"/>
@@ -4743,12 +4967,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427371696"/>
+        <c:crossAx val="347368680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="427371696"/>
+        <c:axId val="347368680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4805,7 +5029,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="352221992"/>
+        <c:crossAx val="347368288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4980,7 +5204,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$M$6</c:f>
+              <c:f>Bangladesh!$M$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5003,7 +5227,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$L$7:$L$62</c:f>
+              <c:f>Bangladesh!$L$7:$L$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -5180,7 +5404,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$M$7:$M$62</c:f>
+              <c:f>Bangladesh!$M$7:$M$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -5362,7 +5586,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$N$6</c:f>
+              <c:f>Bangladesh!$N$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5385,7 +5609,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$L$7:$L$62</c:f>
+              <c:f>Bangladesh!$L$7:$L$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -5562,7 +5786,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$N$7:$N$62</c:f>
+              <c:f>Bangladesh!$N$7:$N$62</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="56"/>
@@ -5747,11 +5971,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="417583776"/>
-        <c:axId val="419597240"/>
+        <c:axId val="421655200"/>
+        <c:axId val="421655592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="417583776"/>
+        <c:axId val="421655200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5808,12 +6032,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="419597240"/>
+        <c:crossAx val="421655592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="419597240"/>
+        <c:axId val="421655592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5870,7 +6094,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417583776"/>
+        <c:crossAx val="421655200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5924,10 +6148,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -6045,7 +6266,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$O$6</c:f>
+              <c:f>Bangladesh!$O$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6068,7 +6289,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$L$7:$L$62</c:f>
+              <c:f>Bangladesh!$L$7:$L$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -6245,7 +6466,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$O$7:$O$62</c:f>
+              <c:f>Bangladesh!$O$7:$O$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -6427,7 +6648,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$P$6</c:f>
+              <c:f>Bangladesh!$P$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6450,7 +6671,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$L$7:$L$62</c:f>
+              <c:f>Bangladesh!$L$7:$L$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -6627,7 +6848,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ECDC Case Death Sheet for Curve'!$P$7:$P$62</c:f>
+              <c:f>Bangladesh!$P$7:$P$62</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="56"/>
@@ -6812,11 +7033,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="427370912"/>
-        <c:axId val="419366424"/>
+        <c:axId val="347367896"/>
+        <c:axId val="347367504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="427370912"/>
+        <c:axId val="347367896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6873,12 +7094,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="419366424"/>
+        <c:crossAx val="347367504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="419366424"/>
+        <c:axId val="347367504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6935,7 +7156,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427370912"/>
+        <c:crossAx val="347367896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6989,7 +7210,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:srgbClr val="FF0000"/>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -10803,10 +11024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:AB62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10815,6 +11036,11 @@
     <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.44140625" customWidth="1"/>
     <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5546875" customWidth="1"/>
+    <col min="19" max="19" width="13.109375" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="24" max="24" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -12352,7 +12578,7 @@
         <v>3.7024504647118426</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>80</v>
       </c>
@@ -12405,7 +12631,7 @@
         <v>4.0615334341282754</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>81</v>
       </c>
@@ -12457,8 +12683,20 @@
         <f t="shared" si="5"/>
         <v>4.4332960821811636</v>
       </c>
+      <c r="S34" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="T34" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="U34" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="V34" s="14" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>82</v>
       </c>
@@ -12510,8 +12748,20 @@
         <f t="shared" si="5"/>
         <v>4.8155240918049156</v>
       </c>
+      <c r="S35" t="s">
+        <v>51</v>
+      </c>
+      <c r="T35" s="17">
+        <v>15</v>
+      </c>
+      <c r="U35" s="17">
+        <v>40</v>
+      </c>
+      <c r="V35" s="17">
+        <v>1250</v>
+      </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>83</v>
       </c>
@@ -12563,8 +12813,23 @@
         <f t="shared" si="5"/>
         <v>5.2057940086691561</v>
       </c>
+      <c r="S36" t="s">
+        <v>10</v>
+      </c>
+      <c r="T36" s="17">
+        <v>60</v>
+      </c>
+      <c r="U36" s="17">
+        <v>20</v>
+      </c>
+      <c r="V36" s="17">
+        <v>410</v>
+      </c>
+      <c r="W36" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>84</v>
       </c>
@@ -12616,8 +12881,23 @@
         <f t="shared" si="5"/>
         <v>5.6015189777685324</v>
       </c>
+      <c r="S37" t="s">
+        <v>13</v>
+      </c>
+      <c r="T37" s="17">
+        <v>130</v>
+      </c>
+      <c r="U37" s="17">
+        <v>40</v>
+      </c>
+      <c r="V37" s="17">
+        <v>880</v>
+      </c>
+      <c r="W37" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>85</v>
       </c>
@@ -12669,8 +12949,26 @@
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
+      <c r="S38" t="s">
+        <v>55</v>
+      </c>
+      <c r="T38" s="11">
+        <f>+'Population by Age and Sex'!D27/1000000</f>
+        <v>15.061970000000001</v>
+      </c>
+      <c r="U38" s="11">
+        <f>+'Population by Age and Sex'!D28/1000000</f>
+        <v>118.212227</v>
+      </c>
+      <c r="V38" s="11">
+        <f>+'Population by Age and Sex'!D26/1000000</f>
+        <v>10.769500000000001</v>
+      </c>
+      <c r="W38" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>86</v>
       </c>
@@ -12722,8 +13020,20 @@
         <f t="shared" si="5"/>
         <v>6.3984810222314668</v>
       </c>
+      <c r="T39" s="17">
+        <v>12</v>
+      </c>
+      <c r="U39" s="17">
+        <v>12</v>
+      </c>
+      <c r="V39" s="17">
+        <v>12</v>
+      </c>
+      <c r="W39" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>87</v>
       </c>
@@ -12775,8 +13085,17 @@
         <f t="shared" si="5"/>
         <v>6.7942059913308439</v>
       </c>
+      <c r="S40" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>88</v>
       </c>
@@ -12828,8 +13147,34 @@
         <f t="shared" si="5"/>
         <v>7.1844759081950844</v>
       </c>
+      <c r="S41" t="s">
+        <v>51</v>
+      </c>
+      <c r="T41" s="12">
+        <f>+T35*T$38*(T$39/12)</f>
+        <v>225.92955000000001</v>
+      </c>
+      <c r="U41" s="12">
+        <f>+U35*U$38*(U$39/12)</f>
+        <v>4728.4890800000003</v>
+      </c>
+      <c r="V41" s="12">
+        <f>+V35*V$38*(V$39/12)</f>
+        <v>13461.875000000002</v>
+      </c>
+      <c r="W41" s="9">
+        <f>SUM(T41:V41)</f>
+        <v>18416.29363</v>
+      </c>
+      <c r="X41" s="12">
+        <f>W41/12</f>
+        <v>1534.6911358333334</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>89</v>
       </c>
@@ -12881,8 +13226,41 @@
         <f t="shared" si="5"/>
         <v>7.5667039178188373</v>
       </c>
+      <c r="S42" t="s">
+        <v>10</v>
+      </c>
+      <c r="T42" s="12">
+        <f>+T36*T$38*(T$39/12)</f>
+        <v>903.71820000000002</v>
+      </c>
+      <c r="U42" s="12">
+        <f t="shared" ref="U42:U43" si="9">+U36*U$38*(U$39/12)</f>
+        <v>2364.2445400000001</v>
+      </c>
+      <c r="V42" s="12">
+        <f>+V36*V$38*(V$39/12)</f>
+        <v>4415.4949999999999</v>
+      </c>
+      <c r="W42" s="9">
+        <f t="shared" ref="W42:W43" si="10">SUM(T42:V42)</f>
+        <v>7683.4577399999998</v>
+      </c>
+      <c r="X42" s="12">
+        <f>W42/12</f>
+        <v>640.28814499999999</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA42">
+        <v>6097</v>
+      </c>
+      <c r="AB42" s="19">
+        <f>AA42/12</f>
+        <v>508.08333333333331</v>
+      </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>90</v>
       </c>
@@ -12934,8 +13312,41 @@
         <f t="shared" si="5"/>
         <v>7.9384665658717237</v>
       </c>
+      <c r="S43" t="s">
+        <v>13</v>
+      </c>
+      <c r="T43" s="12">
+        <f>+T37*T$38*(T$39/12)</f>
+        <v>1958.0561</v>
+      </c>
+      <c r="U43" s="12">
+        <f t="shared" si="9"/>
+        <v>4728.4890800000003</v>
+      </c>
+      <c r="V43" s="12">
+        <f>+V37*V$38*(V$39/12)</f>
+        <v>9477.16</v>
+      </c>
+      <c r="W43" s="9">
+        <f t="shared" si="10"/>
+        <v>16163.705180000001</v>
+      </c>
+      <c r="X43" s="12">
+        <f>W43/12</f>
+        <v>1346.9754316666667</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA43">
+        <v>16804</v>
+      </c>
+      <c r="AB43" s="19">
+        <f>AA43/12</f>
+        <v>1400.3333333333333</v>
+      </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>91</v>
       </c>
@@ -12988,7 +13399,7 @@
         <v>8.297549535288157</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>92</v>
       </c>
@@ -13040,8 +13451,11 @@
         <f t="shared" si="5"/>
         <v>8.6419864368035313</v>
       </c>
+      <c r="V45" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>93</v>
       </c>
@@ -13093,8 +13507,11 @@
         <f t="shared" si="5"/>
         <v>8.9700895494369242</v>
       </c>
+      <c r="V46" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>94</v>
       </c>
@@ -13146,8 +13563,11 @@
         <f t="shared" si="5"/>
         <v>9.2804717714775808</v>
       </c>
+      <c r="S47" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>95</v>
       </c>
@@ -13199,8 +13619,26 @@
         <f t="shared" si="5"/>
         <v>9.5720594284362832</v>
       </c>
+      <c r="S48" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="T48" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="U48" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="V48" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="W48" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="X48" s="24" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>96</v>
       </c>
@@ -13252,8 +13690,28 @@
         <f t="shared" si="5"/>
         <v>9.8440959700225754</v>
       </c>
+      <c r="S49">
+        <v>2017</v>
+      </c>
+      <c r="T49" s="25">
+        <v>3.85E-2</v>
+      </c>
+      <c r="U49" s="18">
+        <v>30354</v>
+      </c>
+      <c r="V49" s="19">
+        <f>U49/T49</f>
+        <v>788415.58441558445</v>
+      </c>
+      <c r="W49" s="10">
+        <v>162</v>
+      </c>
+      <c r="X49" s="19">
+        <f>+V49/W49</f>
+        <v>4866.7628667628669</v>
+      </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>97</v>
       </c>
@@ -13306,7 +13764,7 @@
         <v>10.096136952822516</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>98</v>
       </c>
@@ -13359,7 +13817,7 @@
         <v>10.328037030604534</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>99</v>
       </c>
@@ -13412,7 +13870,7 @@
         <v>10.539929945107424</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>101</v>
       </c>
@@ -13465,7 +13923,7 @@
         <v>10.905465363289586</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>102</v>
       </c>
@@ -13518,7 +13976,7 @@
         <v>11.060517557462191</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>103</v>
       </c>
@@ -13571,7 +14029,7 @@
         <v>11.198313584773704</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>104</v>
       </c>
@@ -13624,7 +14082,7 @@
         <v>11.319926944682845</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>105</v>
       </c>
@@ -13677,7 +14135,7 @@
         <v>11.426515772726223</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>106</v>
       </c>
@@ -13730,7 +14188,7 @@
         <v>11.519290117634196</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>107</v>
       </c>
@@ -13783,7 +14241,7 @@
         <v>11.599481908982193</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>108</v>
       </c>
@@ -13836,7 +14294,7 @@
         <v>11.668318244483876</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>109</v>
       </c>
@@ -13889,7 +14347,7 @@
         <v>11.72699841662185</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>110</v>
       </c>
@@ -13943,7 +14401,466 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="W36" r:id="rId1"/>
+    <hyperlink ref="V45" r:id="rId2"/>
+    <hyperlink ref="V46" r:id="rId3"/>
+    <hyperlink ref="S47" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="7">
+        <v>72109796</v>
+      </c>
+      <c r="C4" s="7">
+        <v>71933901</v>
+      </c>
+      <c r="D4" s="7">
+        <v>144043697</v>
+      </c>
+      <c r="E4" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="7">
+        <v>7638523</v>
+      </c>
+      <c r="C5" s="7">
+        <v>7423447</v>
+      </c>
+      <c r="D5" s="7">
+        <v>15061970</v>
+      </c>
+      <c r="E5" s="6">
+        <v>10.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="7">
+        <v>9322514</v>
+      </c>
+      <c r="C6" s="7">
+        <v>8850715</v>
+      </c>
+      <c r="D6" s="7">
+        <v>18173229</v>
+      </c>
+      <c r="E6" s="6">
+        <v>12.62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="7">
+        <v>8614889</v>
+      </c>
+      <c r="C7" s="7">
+        <v>8031726</v>
+      </c>
+      <c r="D7" s="7">
+        <v>16646615</v>
+      </c>
+      <c r="E7" s="6">
+        <v>11.56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="7">
+        <v>6509492</v>
+      </c>
+      <c r="C8" s="7">
+        <v>6352398</v>
+      </c>
+      <c r="D8" s="7">
+        <v>12861890</v>
+      </c>
+      <c r="E8" s="6">
+        <v>8.93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="7">
+        <v>5777370</v>
+      </c>
+      <c r="C9" s="7">
+        <v>7522419</v>
+      </c>
+      <c r="D9" s="7">
+        <v>13299789</v>
+      </c>
+      <c r="E9" s="6">
+        <v>9.23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="7">
+        <v>6225252</v>
+      </c>
+      <c r="C10" s="7">
+        <v>7254256</v>
+      </c>
+      <c r="D10" s="7">
+        <v>13479508</v>
+      </c>
+      <c r="E10" s="6">
+        <v>9.36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="7">
+        <v>5079106</v>
+      </c>
+      <c r="C11" s="7">
+        <v>5420659</v>
+      </c>
+      <c r="D11" s="7">
+        <v>10499765</v>
+      </c>
+      <c r="E11" s="6">
+        <v>7.29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="7">
+        <v>4697349</v>
+      </c>
+      <c r="C12" s="7">
+        <v>4859079</v>
+      </c>
+      <c r="D12" s="7">
+        <v>9556428</v>
+      </c>
+      <c r="E12" s="6">
+        <v>6.63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="7">
+        <v>4280923</v>
+      </c>
+      <c r="C13" s="7">
+        <v>3980739</v>
+      </c>
+      <c r="D13" s="7">
+        <v>8261662</v>
+      </c>
+      <c r="E13" s="6">
+        <v>5.74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="7">
+        <v>3363273</v>
+      </c>
+      <c r="C14" s="7">
+        <v>3016800</v>
+      </c>
+      <c r="D14" s="7">
+        <v>6380073</v>
+      </c>
+      <c r="E14" s="6">
+        <v>4.43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="7">
+        <v>2952596</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2599675</v>
+      </c>
+      <c r="D15" s="7">
+        <v>5552271</v>
+      </c>
+      <c r="E15" s="6">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="7">
+        <v>1923534</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1577463</v>
+      </c>
+      <c r="D16" s="7">
+        <v>3500997</v>
+      </c>
+      <c r="E16" s="6">
+        <v>2.4300000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="7">
+        <v>2081306</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1852708</v>
+      </c>
+      <c r="D17" s="7">
+        <v>3934014</v>
+      </c>
+      <c r="E17" s="6">
+        <v>2.73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1149569</v>
+      </c>
+      <c r="C18" s="7">
+        <v>963921</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2113490</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="7">
+        <v>1206398</v>
+      </c>
+      <c r="C19" s="7">
+        <v>1025314</v>
+      </c>
+      <c r="D19" s="7">
+        <v>2231712</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="7">
+        <v>488338</v>
+      </c>
+      <c r="C20" s="7">
+        <v>386389</v>
+      </c>
+      <c r="D20" s="7">
+        <v>874727</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="7">
+        <v>443239</v>
+      </c>
+      <c r="C21" s="7">
+        <v>436840</v>
+      </c>
+      <c r="D21" s="7">
+        <v>880079</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="7">
+        <v>138268</v>
+      </c>
+      <c r="C22" s="7">
+        <v>124343</v>
+      </c>
+      <c r="D22" s="7">
+        <v>262611</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="7">
+        <v>116916</v>
+      </c>
+      <c r="C23" s="7">
+        <v>133273</v>
+      </c>
+      <c r="D23" s="7">
+        <v>250189</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="7">
+        <v>100941</v>
+      </c>
+      <c r="C24" s="7">
+        <v>121737</v>
+      </c>
+      <c r="D24" s="7">
+        <v>222678</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="8">
+        <f>SUM(B17:B24)</f>
+        <v>5724975</v>
+      </c>
+      <c r="C26" s="8">
+        <f t="shared" ref="C26:D26" si="0">SUM(C17:C24)</f>
+        <v>5044525</v>
+      </c>
+      <c r="D26" s="8">
+        <f t="shared" si="0"/>
+        <v>10769500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="8">
+        <f>+B5</f>
+        <v>7638523</v>
+      </c>
+      <c r="C27" s="8">
+        <f t="shared" ref="C27:D27" si="1">+C5</f>
+        <v>7423447</v>
+      </c>
+      <c r="D27" s="8">
+        <f t="shared" si="1"/>
+        <v>15061970</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="8">
+        <f>SUM(B6:B16)</f>
+        <v>58746298</v>
+      </c>
+      <c r="C28" s="8">
+        <f t="shared" ref="C28:D28" si="2">SUM(C6:C16)</f>
+        <v>59465929</v>
+      </c>
+      <c r="D28" s="8">
+        <f t="shared" si="2"/>
+        <v>118212227</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>